<commit_message>
updated TP-Candidate Registration files
</commit_message>
<xml_diff>
--- a/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
+++ b/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="185">
   <si>
     <t>Common Candidate Details</t>
   </si>
@@ -445,9 +445,6 @@
     <t>Married</t>
   </si>
   <si>
-    <t>ID123456</t>
-  </si>
-  <si>
     <t>OBC</t>
   </si>
   <si>
@@ -550,16 +547,28 @@
     <t>MotherName</t>
   </si>
   <si>
-    <t>NewBulkA</t>
-  </si>
-  <si>
-    <t>NewBulkB</t>
-  </si>
-  <si>
-    <t>NewBulkC</t>
-  </si>
-  <si>
-    <t>NewBulkD</t>
+    <t>NewPBulkA</t>
+  </si>
+  <si>
+    <t>NewPBulkB</t>
+  </si>
+  <si>
+    <t>NewPBulkC</t>
+  </si>
+  <si>
+    <t>NewPBulkD</t>
+  </si>
+  <si>
+    <t>ID123458</t>
+  </si>
+  <si>
+    <t>ID123459</t>
+  </si>
+  <si>
+    <t>ID123476</t>
+  </si>
+  <si>
+    <t>ID123486</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1150,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5"/>
@@ -5690,10 +5699,10 @@
         <v>130</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>136</v>
@@ -5702,55 +5711,58 @@
         <v>138</v>
       </c>
       <c r="F5" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="H5" s="29" t="s">
-        <v>177</v>
+      <c r="L5" s="28" t="s">
+        <v>181</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N5" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="O5" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="O5" s="29" t="s">
-        <v>148</v>
-      </c>
       <c r="P5" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q5" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R5" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S5" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T5" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U5" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W5" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X5" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y5" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z5" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA5" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB5" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:1025">
@@ -5758,7 +5770,7 @@
         <v>131</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>133</v>
@@ -5770,58 +5782,58 @@
         <v>139</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I6" s="28" t="s">
         <v>34</v>
       </c>
       <c r="L6" s="28" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N6" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O6" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P6" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q6" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R6" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S6" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T6" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U6" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W6" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X6" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Y6" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Z6" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AA6" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AB6" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:1025">
@@ -5829,7 +5841,7 @@
         <v>132</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>135</v>
@@ -5841,58 +5853,58 @@
         <v>140</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I7" s="28" t="s">
         <v>34</v>
       </c>
       <c r="L7" s="28" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="M7" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="N7" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="N7" s="29" t="s">
-        <v>147</v>
-      </c>
       <c r="O7" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P7" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q7" s="28" t="s">
         <v>140</v>
       </c>
       <c r="R7" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S7" s="28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="T7" s="28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U7" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="W7" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="X7" s="28" t="s">
         <v>140</v>
       </c>
       <c r="Y7" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Z7" s="28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AA7" s="28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AB7" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:1025">
@@ -5900,7 +5912,7 @@
         <v>129</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>134</v>
@@ -5918,52 +5930,52 @@
         <v>34</v>
       </c>
       <c r="L8" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="M8" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="M8" s="29" t="s">
-        <v>144</v>
-      </c>
       <c r="N8" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O8" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P8" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R8" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S8" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T8" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U8" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="W8" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="X8" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Y8" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Z8" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AA8" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AB8" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated TP-BulkCandidate Test Data File
</commit_message>
<xml_diff>
--- a/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
+++ b/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="186">
   <si>
     <t>Common Candidate Details</t>
   </si>
@@ -457,9 +457,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Muslim</t>
-  </si>
-  <si>
     <t>Christian</t>
   </si>
   <si>
@@ -547,18 +544,6 @@
     <t>MotherName</t>
   </si>
   <si>
-    <t>NewPBulkA</t>
-  </si>
-  <si>
-    <t>NewPBulkB</t>
-  </si>
-  <si>
-    <t>NewPBulkC</t>
-  </si>
-  <si>
-    <t>NewPBulkD</t>
-  </si>
-  <si>
     <t>ID123458</t>
   </si>
   <si>
@@ -569,6 +554,24 @@
   </si>
   <si>
     <t>ID123486</t>
+  </si>
+  <si>
+    <t>NewPalsVpBulkC</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Hindu</t>
+  </si>
+  <si>
+    <t>NewvPalsVpBulkA</t>
+  </si>
+  <si>
+    <t>NewvPalsVpBulkB</t>
+  </si>
+  <si>
+    <t>NewvPalsVpBulkD</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1153,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5"/>
@@ -5699,7 +5702,7 @@
         <v>130</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>134</v>
@@ -5711,58 +5714,64 @@
         <v>138</v>
       </c>
       <c r="F5" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="I5" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="28" t="s">
         <v>176</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>181</v>
       </c>
       <c r="M5" s="29" t="s">
         <v>143</v>
       </c>
       <c r="N5" s="29" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O5" s="29" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P5" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Q5" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R5" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S5" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T5" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="U5" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W5" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="X5" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y5" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z5" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA5" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AB5" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:1025">
@@ -5770,10 +5779,10 @@
         <v>131</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>136</v>
@@ -5782,13 +5791,19 @@
         <v>139</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>175</v>
       </c>
       <c r="I6" s="28" t="s">
         <v>34</v>
       </c>
       <c r="L6" s="28" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="M6" s="29" t="s">
         <v>144</v>
@@ -5797,43 +5812,43 @@
         <v>146</v>
       </c>
       <c r="O6" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P6" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q6" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R6" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S6" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T6" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U6" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W6" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X6" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y6" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z6" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA6" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB6" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:1025">
@@ -5841,10 +5856,10 @@
         <v>132</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>136</v>
@@ -5853,13 +5868,19 @@
         <v>140</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>175</v>
       </c>
       <c r="I7" s="28" t="s">
         <v>34</v>
       </c>
       <c r="L7" s="28" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="M7" s="29" t="s">
         <v>145</v>
@@ -5868,43 +5889,43 @@
         <v>146</v>
       </c>
       <c r="O7" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P7" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q7" s="28" t="s">
         <v>140</v>
       </c>
       <c r="R7" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S7" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T7" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U7" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W7" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X7" s="28" t="s">
         <v>140</v>
       </c>
       <c r="Y7" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Z7" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AA7" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AB7" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:1025">
@@ -5912,7 +5933,7 @@
         <v>129</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>134</v>
@@ -5926,11 +5947,17 @@
       <c r="F8" s="28" t="s">
         <v>142</v>
       </c>
+      <c r="G8" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>175</v>
+      </c>
       <c r="I8" s="28" t="s">
         <v>34</v>
       </c>
       <c r="L8" s="28" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="M8" s="29" t="s">
         <v>143</v>
@@ -5939,43 +5966,43 @@
         <v>146</v>
       </c>
       <c r="O8" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P8" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R8" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S8" s="28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="T8" s="28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U8" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="W8" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="X8" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Y8" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Z8" s="28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AA8" s="28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AB8" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ToT-ToA Batch workflow and TP-Bulk Candidate Registration Excel file.
</commit_message>
<xml_diff>
--- a/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
+++ b/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="174">
   <si>
     <t>Common Candidate Details</t>
   </si>
@@ -438,28 +438,13 @@
     <t>PlacementTrackingDate3</t>
   </si>
   <si>
-    <t>Mr.</t>
-  </si>
-  <si>
-    <t>Dr.</t>
-  </si>
-  <si>
-    <t>Mrs.</t>
-  </si>
-  <si>
-    <t>Ms.</t>
-  </si>
-  <si>
-    <t>finalNewPalsVBulkA</t>
-  </si>
-  <si>
-    <t>finalNewPalsVBulkB</t>
-  </si>
-  <si>
-    <t>finalNewPalsVBulkD</t>
-  </si>
-  <si>
-    <t>finalNewPalsVBulkC</t>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>Ms</t>
   </si>
   <si>
     <t>Male</t>
@@ -471,15 +456,18 @@
     <t>Transgender</t>
   </si>
   <si>
+    <t>25/09/2004</t>
+  </si>
+  <si>
+    <t>04/02/1992</t>
+  </si>
+  <si>
     <t>31/08/2004</t>
   </si>
   <si>
     <t>01/09/2004</t>
   </si>
   <si>
-    <t>04/02/1992</t>
-  </si>
-  <si>
     <t>Kasargod</t>
   </si>
   <si>
@@ -507,6 +495,18 @@
     <t>MotherName</t>
   </si>
   <si>
+    <t>KASARAGOD</t>
+  </si>
+  <si>
+    <t>ANANTAPUR</t>
+  </si>
+  <si>
+    <t>CHITRADURGA</t>
+  </si>
+  <si>
+    <t>NICOBARS</t>
+  </si>
+  <si>
     <t>KERALA</t>
   </si>
   <si>
@@ -519,19 +519,28 @@
     <t>ANDAMAN AND NICOBAR ISLANDS</t>
   </si>
   <si>
-    <t>KASARAGOD</t>
-  </si>
-  <si>
-    <t>ANANTAPUR</t>
-  </si>
-  <si>
-    <t>CHITRADURGA</t>
-  </si>
-  <si>
-    <t>NICOBARS</t>
-  </si>
-  <si>
-    <t>25/09/2004</t>
+    <t>9011223390</t>
+  </si>
+  <si>
+    <t>PalsVpBulkA</t>
+  </si>
+  <si>
+    <t>PalsVpBulkB</t>
+  </si>
+  <si>
+    <t>PalsVpBulkC</t>
+  </si>
+  <si>
+    <t>PalsVpBulkD</t>
+  </si>
+  <si>
+    <t>9011223391</t>
+  </si>
+  <si>
+    <t>9011223392</t>
+  </si>
+  <si>
+    <t>9011223393</t>
   </si>
 </sst>
 </file>
@@ -690,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -763,6 +772,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1138,7 +1148,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1148,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
@@ -1940,139 +1950,151 @@
         <v>139</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="E5" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>153</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>157</v>
       </c>
       <c r="G5" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I5" s="23" t="s">
         <v>35</v>
       </c>
       <c r="V5" s="23" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="X5" s="23" t="s">
         <v>162</v>
+      </c>
+      <c r="AA5" s="26" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:89">
       <c r="A6" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E6" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>154</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>158</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I6" s="23" t="s">
         <v>35</v>
       </c>
       <c r="V6" s="23" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="X6" s="23" t="s">
         <v>163</v>
+      </c>
+      <c r="AA6" s="26" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:89">
       <c r="A7" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E7" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>155</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>159</v>
       </c>
       <c r="G7" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I7" s="23" t="s">
         <v>35</v>
       </c>
       <c r="V7" s="23" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="X7" s="23" t="s">
         <v>164</v>
+      </c>
+      <c r="AA7" s="26" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:89">
       <c r="A8" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>147</v>
-      </c>
       <c r="D8" s="23" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E8" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>156</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>160</v>
       </c>
       <c r="G8" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>35</v>
       </c>
       <c r="V8" s="23" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="X8" s="23" t="s">
         <v>165</v>
+      </c>
+      <c r="AA8" s="26" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated TP- Bulk Candidate Registration, ToT-ToA and Assessor-Trainer test cases.
</commit_message>
<xml_diff>
--- a/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
+++ b/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="204">
   <si>
     <t>Common Candidate Details</t>
   </si>
@@ -522,18 +522,6 @@
     <t>9011223390</t>
   </si>
   <si>
-    <t>PalsVpBulkA</t>
-  </si>
-  <si>
-    <t>PalsVpBulkB</t>
-  </si>
-  <si>
-    <t>PalsVpBulkC</t>
-  </si>
-  <si>
-    <t>PalsVpBulkD</t>
-  </si>
-  <si>
     <t>9011223391</t>
   </si>
   <si>
@@ -541,13 +529,115 @@
   </si>
   <si>
     <t>9011223393</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>OBC</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Hindu</t>
+  </si>
+  <si>
+    <t>Muslim</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Sikh</t>
+  </si>
+  <si>
+    <t>577558</t>
+  </si>
+  <si>
+    <t>577559</t>
+  </si>
+  <si>
+    <t>577557</t>
+  </si>
+  <si>
+    <t>577556</t>
+  </si>
+  <si>
+    <t>pals1@gmail.com</t>
+  </si>
+  <si>
+    <t>pals2@gmail.com</t>
+  </si>
+  <si>
+    <t>pals3@gmail.com</t>
+  </si>
+  <si>
+    <t>pals4@gmail.com</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Kasaragod</t>
+  </si>
+  <si>
+    <t>Hiriyur</t>
+  </si>
+  <si>
+    <t>Chitradurga</t>
+  </si>
+  <si>
+    <t>Anantapur</t>
+  </si>
+  <si>
+    <t>Car Nicobar</t>
+  </si>
+  <si>
+    <t>Andaman and Nicobar Islands</t>
+  </si>
+  <si>
+    <t>#301-306, World Mark 1, West Wing, Aerocity</t>
+  </si>
+  <si>
+    <t>PalsVpBulkAA</t>
+  </si>
+  <si>
+    <t>PalsVpBulkBB</t>
+  </si>
+  <si>
+    <t>PalsVpBulkCC</t>
+  </si>
+  <si>
+    <t>PalsVpBulkDD</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>Post Graduate</t>
+  </si>
+  <si>
+    <t>Diploma</t>
+  </si>
+  <si>
+    <t>10th</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -595,6 +685,27 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="63"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -695,11 +806,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -773,9 +888,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1148,7 +1266,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1158,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
@@ -1945,12 +2063,12 @@
       <c r="CJ4" s="22"/>
       <c r="CK4" s="22"/>
     </row>
-    <row r="5" spans="1:89">
+    <row r="5" spans="1:89" ht="15.5">
       <c r="A5" s="23" t="s">
         <v>139</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>167</v>
+        <v>196</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>142</v>
@@ -1973,22 +2091,73 @@
       <c r="I5" s="23" t="s">
         <v>35</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O5" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="P5" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="V5" s="23" t="s">
-        <v>158</v>
+        <v>160</v>
+      </c>
+      <c r="W5" s="26" t="s">
+        <v>180</v>
       </c>
       <c r="X5" s="23" t="s">
-        <v>162</v>
+        <v>164</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="AA5" s="26" t="s">
         <v>166</v>
       </c>
+      <c r="AC5" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
-    <row r="6" spans="1:89">
+    <row r="6" spans="1:89" ht="15.5">
       <c r="A6" s="23" t="s">
         <v>141</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>143</v>
@@ -2011,22 +2180,73 @@
       <c r="I6" s="23" t="s">
         <v>35</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="V6" s="23" t="s">
         <v>159</v>
       </c>
+      <c r="W6" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="X6" s="23" t="s">
         <v>163</v>
       </c>
+      <c r="Y6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="AA6" s="26" t="s">
-        <v>171</v>
+        <v>167</v>
+      </c>
+      <c r="AC6" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:89">
+    <row r="7" spans="1:89" ht="15.5">
       <c r="A7" s="23" t="s">
         <v>140</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>169</v>
+        <v>198</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>144</v>
@@ -2049,22 +2269,73 @@
       <c r="I7" s="23" t="s">
         <v>35</v>
       </c>
+      <c r="J7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q7" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="T7" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="V7" s="23" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="W7" s="26" t="s">
+        <v>182</v>
       </c>
       <c r="X7" s="23" t="s">
-        <v>164</v>
+        <v>162</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="AA7" s="26" t="s">
-        <v>172</v>
+        <v>168</v>
+      </c>
+      <c r="AC7" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:89">
+    <row r="8" spans="1:89" ht="15.5">
       <c r="A8" s="23" t="s">
         <v>141</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>142</v>
@@ -2087,19 +2358,76 @@
       <c r="I8" s="23" t="s">
         <v>35</v>
       </c>
+      <c r="J8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M8" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O8" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q8" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="T8" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="V8" s="23" t="s">
         <v>161</v>
       </c>
+      <c r="W8" s="26" t="s">
+        <v>183</v>
+      </c>
       <c r="X8" s="23" t="s">
         <v>165</v>
       </c>
+      <c r="Y8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="AA8" s="26" t="s">
-        <v>173</v>
+        <v>169</v>
+      </c>
+      <c r="AC8" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AC5" r:id="rId1"/>
+    <hyperlink ref="AC6" r:id="rId2"/>
+    <hyperlink ref="AC7" r:id="rId3"/>
+    <hyperlink ref="AC8" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Updated ToT-ToA, Assessor-Trainer ans TP-Candididate Workflow test cases.
</commit_message>
<xml_diff>
--- a/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
+++ b/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="208">
   <si>
     <t>Common Candidate Details</t>
   </si>
@@ -468,18 +468,12 @@
     <t>01/09/2004</t>
   </si>
   <si>
-    <t>Kasargod</t>
-  </si>
-  <si>
     <t>Anantpur</t>
   </si>
   <si>
     <t>Aimangala</t>
   </si>
   <si>
-    <t>Aadivala</t>
-  </si>
-  <si>
     <t>Single</t>
   </si>
   <si>
@@ -609,18 +603,6 @@
     <t>#301-306, World Mark 1, West Wing, Aerocity</t>
   </si>
   <si>
-    <t>PalsVpBulkAA</t>
-  </si>
-  <si>
-    <t>PalsVpBulkBB</t>
-  </si>
-  <si>
-    <t>PalsVpBulkCC</t>
-  </si>
-  <si>
-    <t>PalsVpBulkDD</t>
-  </si>
-  <si>
     <t>Graduate</t>
   </si>
   <si>
@@ -631,13 +613,43 @@
   </si>
   <si>
     <t>10th</t>
+  </si>
+  <si>
+    <t>#401-406, World Mark 1, West Wing, Aerocity</t>
+  </si>
+  <si>
+    <t>TAMIL NADU</t>
+  </si>
+  <si>
+    <t>TIRUNELVELI</t>
+  </si>
+  <si>
+    <t>Tirunelveli</t>
+  </si>
+  <si>
+    <t>677558</t>
+  </si>
+  <si>
+    <t>Big Lapati</t>
+  </si>
+  <si>
+    <t>PalsVpBulkTRA</t>
+  </si>
+  <si>
+    <t>PalsVpBulkTRB</t>
+  </si>
+  <si>
+    <t>PalsVpBulkTRC</t>
+  </si>
+  <si>
+    <t>PalsVpBulkTRD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -707,6 +719,12 @@
       <sz val="12"/>
       <color indexed="63"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -814,7 +832,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -890,6 +908,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1266,7 +1285,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1276,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
@@ -2068,7 +2087,7 @@
         <v>139</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>142</v>
@@ -2077,79 +2096,79 @@
         <v>145</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G5" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I5" s="23" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="M5" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O5" s="23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P5" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="U5" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="V5" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="W5" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="X5" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y5" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA5" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="Q5" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="T5" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="V5" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="W5" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="X5" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA5" s="26" t="s">
-        <v>166</v>
-      </c>
       <c r="AC5" s="27" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:89" ht="15.5">
@@ -2157,7 +2176,7 @@
         <v>141</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>143</v>
@@ -2166,79 +2185,79 @@
         <v>146</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I6" s="23" t="s">
         <v>35</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="M6" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="V6" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="W6" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="X6" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA6" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC6" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="AF6" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="O6" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="P6" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q6" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="T6" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="V6" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="W6" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="X6" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA6" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="AC6" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="AF6" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:89" ht="15.5">
@@ -2246,7 +2265,7 @@
         <v>140</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>144</v>
@@ -2254,80 +2273,80 @@
       <c r="D7" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>151</v>
+      <c r="E7" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G7" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I7" s="23" t="s">
         <v>35</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M7" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="O7" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P7" s="23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q7" s="26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="T7" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="V7" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="W7" s="26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="X7" s="23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AA7" s="26" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AC7" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="AF7" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:89" ht="15.5">
@@ -2335,7 +2354,7 @@
         <v>141</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>142</v>
@@ -2344,79 +2363,79 @@
         <v>148</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>152</v>
+        <v>203</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G8" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>35</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M8" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="O8" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q8" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="T8" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="O8" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q8" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="T8" s="28" t="s">
-        <v>195</v>
-      </c>
       <c r="U8" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="V8" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="W8" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="X8" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AA8" s="26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AC8" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated TP- BulkCandidateRegistration excel template file
</commit_message>
<xml_diff>
--- a/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
+++ b/NSDC_Web_Automation/UploadFiles/BulkCandidatesRegistrationByTP.xlsx
@@ -474,9 +474,6 @@
     <t>Aimangala</t>
   </si>
   <si>
-    <t>Single</t>
-  </si>
-  <si>
     <t>Divorcee</t>
   </si>
   <si>
@@ -643,13 +640,16 @@
   </si>
   <si>
     <t>PalsVpBulkTRD</t>
+  </si>
+  <si>
+    <t>Single/Unmarried</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -724,6 +724,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -832,7 +837,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -909,6 +914,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1285,7 +1291,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1296,7 +1302,7 @@
   <dimension ref="A1:AMG8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
@@ -2087,7 +2093,7 @@
         <v>139</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>142</v>
@@ -2098,77 +2104,77 @@
       <c r="E5" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>151</v>
+      <c r="F5" s="30" t="s">
+        <v>207</v>
       </c>
       <c r="G5" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I5" s="23" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M5" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O5" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="P5" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="U5" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="V5" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="W5" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="X5" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y5" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AA5" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC5" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF5" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="O5" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="P5" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q5" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="T5" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="U5" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="V5" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="W5" s="26" t="s">
-        <v>202</v>
-      </c>
-      <c r="X5" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="Y5" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AA5" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="AC5" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:89" ht="15.5">
@@ -2176,7 +2182,7 @@
         <v>141</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>143</v>
@@ -2188,76 +2194,76 @@
         <v>149</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I6" s="23" t="s">
         <v>35</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M6" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O6" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P6" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T6" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="V6" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="W6" s="26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="X6" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AA6" s="26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AC6" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:89" ht="15.5">
@@ -2265,7 +2271,7 @@
         <v>140</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>144</v>
@@ -2274,79 +2280,79 @@
         <v>147</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G7" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I7" s="23" t="s">
         <v>35</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M7" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O7" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P7" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q7" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="T7" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="T7" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="V7" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="W7" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="X7" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AA7" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC7" s="27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF7" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:89" ht="15.5">
@@ -2354,7 +2360,7 @@
         <v>141</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>142</v>
@@ -2363,79 +2369,79 @@
         <v>148</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G8" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>35</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M8" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N8" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O8" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q8" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O8" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q8" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="T8" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="T8" s="28" t="s">
-        <v>193</v>
-      </c>
       <c r="U8" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="V8" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="W8" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="X8" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y8" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="V8" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="W8" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="X8" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="Z8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AA8" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC8" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>